<commit_message>
Changed 12-24 ATA Factor
Changed to simple average because...
</commit_message>
<xml_diff>
--- a/RAA.xlsx
+++ b/RAA.xlsx
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1066,16 +1066,16 @@
         <v>2063</v>
       </c>
       <c r="O11" s="4">
-        <f>B15</f>
-        <v>2.9993586513353794</v>
+        <f>B29</f>
+        <v>8.2060992795413554</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="1"/>
-        <v>9.0094362357200009</v>
+        <v>24.649379016443866</v>
       </c>
       <c r="Q11" s="5">
         <f t="shared" si="0"/>
-        <v>18586.466954290361</v>
+        <v>50851.668910923698</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="Q13" s="5">
         <f>SUM(Q2:Q12)</f>
-        <v>215253.45054382225</v>
+        <v>247518.65250045559</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "Changed 12-24 ATA Factor"
This reverts commit 2e34b50deb82b4cd2a05a883c27be08a32f76c2e.
</commit_message>
<xml_diff>
--- a/RAA.xlsx
+++ b/RAA.xlsx
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1066,16 +1066,16 @@
         <v>2063</v>
       </c>
       <c r="O11" s="4">
-        <f>B29</f>
-        <v>8.2060992795413554</v>
+        <f>B15</f>
+        <v>2.9993586513353794</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="1"/>
-        <v>24.649379016443866</v>
+        <v>9.0094362357200009</v>
       </c>
       <c r="Q11" s="5">
         <f t="shared" si="0"/>
-        <v>50851.668910923698</v>
+        <v>18586.466954290361</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="Q13" s="5">
         <f>SUM(Q2:Q12)</f>
-        <v>247518.65250045559</v>
+        <v>215253.45054382225</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>